<commit_message>
Corrigindo a planilha de Cronograma
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\treinamento\devsuperior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2192EBD9-BD17-44EB-8536-0645000EDB87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB517995-4D8D-4495-950B-42776F7207BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B6EC0019-EB5A-4F6F-9E45-13B4089E443E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E553424B-E5F1-411E-8A93-C12E35D2C412}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Manhã</t>
   </si>
@@ -45,6 +45,9 @@
     <t>Noite</t>
   </si>
   <si>
+    <t>Domingo</t>
+  </si>
+  <si>
     <t>Segunda</t>
   </si>
   <si>
@@ -63,10 +66,10 @@
     <t>Sábado</t>
   </si>
   <si>
-    <t>Domingo</t>
-  </si>
-  <si>
-    <t>CRONOGRAMA DE ESTUDOS DEVSUPERIOR</t>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -82,15 +85,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="22"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,13 +101,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,23 +133,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,104 +456,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100683BB-B774-4168-B769-27C816CF4045}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5B72EC-E593-4E74-8639-08DFC138303D}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="15" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2">
-        <v>4</v>
-      </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:H1"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>